<commit_message>
gemini feedback - v0.4
</commit_message>
<xml_diff>
--- a/docs/research/t_ele_zi-20251127.xlsx
+++ b/docs/research/t_ele_zi-20251127.xlsx
@@ -88,7 +88,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">治理 </t>
@@ -98,13 +98,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/ </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">交错</t>
@@ -141,7 +142,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">植物</t>
@@ -151,6 +152,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -177,7 +179,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">概念</t>
@@ -187,6 +189,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -471,7 +474,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">社会</t>
@@ -481,6 +484,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -663,7 +667,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">动物</t>
@@ -673,6 +677,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -735,7 +740,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天文</t>
@@ -745,13 +750,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">木</t>
@@ -806,7 +812,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">地理</t>
@@ -816,6 +822,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -826,13 +833,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">indicates a place or location (like in </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">邓</t>
@@ -842,13 +850,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/dèng, </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">邻</t>
@@ -858,13 +867,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/lín, </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">都</t>
@@ -874,6 +884,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/dū).</t>
     </r>
@@ -900,7 +911,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">人</t>
@@ -910,13 +921,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">行</t>
@@ -950,7 +962,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">人</t>
@@ -960,13 +972,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">伦理</t>
@@ -1111,7 +1124,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">数理</t>
@@ -1121,13 +1134,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">时空</t>
@@ -1212,7 +1226,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">数理</t>
@@ -1222,13 +1236,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天干</t>
@@ -1277,7 +1292,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天文</t>
@@ -1287,6 +1302,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -1370,7 +1386,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">数理</t>
@@ -1380,13 +1396,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">计算</t>
@@ -1401,13 +1418,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">sounds similar to </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">久 </t>
@@ -1417,6 +1435,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(jiǔ), which means "long-lasting" or "eternal."</t>
     </r>
@@ -1451,13 +1470,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> able-bodied men / fourth of the ten Heavenly Stems (</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天干</t>
@@ -1467,6 +1487,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -1793,7 +1814,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">社会</t>
@@ -1803,13 +1824,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">文化</t>
@@ -1980,13 +2002,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">first of the ten Heavenly Stems (</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天干</t>
@@ -1996,6 +2019,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">) / shell / armor / first / top</t>
     </r>
@@ -2028,7 +2052,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">数理</t>
@@ -2038,13 +2062,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">度量</t>
@@ -2429,7 +2454,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">人</t>
@@ -2439,13 +2464,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">生理</t>
@@ -2527,7 +2553,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天文</t>
@@ -2537,13 +2563,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">水</t>
@@ -2631,7 +2658,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">人</t>
@@ -2641,13 +2668,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">心理</t>
@@ -2794,13 +2822,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"tenth of the ten Heavenly Stems </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">十天干</t>
@@ -2810,6 +2839,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[shi2 tian1 gan1]/tenth in order/letter ""J"" or Roman ""X"" in list ""A, B, C"", or ""I, II, III"" etc/ancient Chinese compass point: 15°/deca"</t>
     </r>
@@ -2836,7 +2866,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">社会</t>
@@ -2846,13 +2876,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">军事</t>
@@ -2874,7 +2905,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">动物</t>
@@ -2884,13 +2915,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">生肖</t>
@@ -2972,7 +3004,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">地理</t>
@@ -2982,13 +3014,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">土</t>
@@ -3294,13 +3327,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">fifth of the ten Heavenly Stems </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">十天干</t>
@@ -3310,6 +3344,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[shi2 tian1 gan1]/fifth in order/letter ""E"" or Roman ""V"" in list ""A, B, C"", or ""I, II, III"" etc/penta"</t>
     </r>
@@ -3453,7 +3488,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">数理</t>
@@ -3463,13 +3498,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">颜色</t>
@@ -4256,7 +4292,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">社会</t>
@@ -4266,13 +4302,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">商业</t>
@@ -4468,7 +4505,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">人</t>
@@ -4478,6 +4515,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
@@ -4933,7 +4971,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">囚、四、國、圍 回 </t>
@@ -4943,13 +4981,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(huí), </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">国 </t>
@@ -4959,13 +4998,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(guó), and </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">园 </t>
@@ -4975,6 +5015,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(yuán)</t>
     </r>
@@ -5001,7 +5042,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天文</t>
@@ -5011,13 +5052,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">土</t>
@@ -5162,7 +5204,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">人</t>
@@ -5172,13 +5214,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">住</t>
@@ -5263,7 +5306,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">艸</t>
@@ -5273,13 +5316,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">草</t>
@@ -5379,7 +5423,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">人</t>
@@ -5389,13 +5433,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">衣</t>
@@ -5531,7 +5576,7 @@
     <t xml:space="preserve">彐</t>
   </si>
   <si>
-    <t xml:space="preserve">garment / snout</t>
+    <t xml:space="preserve">garment / snout / broom</t>
   </si>
   <si>
     <t xml:space="preserve">jì / tiáo</t>
@@ -5540,7 +5585,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">录 </t>
@@ -5550,13 +5595,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(lù) and </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">彖 </t>
@@ -5566,13 +5612,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(tuàn)</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">、彗</t>
@@ -5606,7 +5653,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">形 </t>
@@ -5616,13 +5663,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(xíng, shape/form) and </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">彩 </t>
@@ -5632,13 +5680,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(cǎi, color/variety)</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">、彤、彥</t>
@@ -5666,7 +5715,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">行 </t>
@@ -5676,13 +5725,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(xíng, to walk/travel), </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">往 </t>
@@ -5692,13 +5742,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(wǎng, to go), and </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">德 </t>
@@ -5708,13 +5759,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(dé, virtue/morality)</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">、彷</t>
@@ -5964,7 +6016,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天文</t>
@@ -5974,13 +6026,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">日</t>
@@ -6092,7 +6145,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">段 </t>
@@ -6102,13 +6155,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(duàn) and </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">般 </t>
@@ -6118,13 +6172,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(bān)</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">、殷、殺</t>
@@ -6287,7 +6342,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天文</t>
@@ -6297,13 +6352,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">火</t>
@@ -6315,13 +6371,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">means water when appearing in </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">魚</t>
@@ -6706,7 +6763,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">癸、癹、発 </t>
@@ -6716,13 +6773,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">發</t>
@@ -6900,7 +6958,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">人</t>
@@ -6910,13 +6968,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">食</t>
@@ -7214,7 +7273,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天文</t>
@@ -7224,13 +7283,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">月</t>
@@ -7240,13 +7300,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">人</t>
@@ -7256,13 +7317,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">生理</t>
@@ -7829,13 +7891,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">city (</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">阝 </t>
@@ -7845,6 +7908,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">right)</t>
     </r>
@@ -7880,7 +7944,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">采、釉、釋 </t>
@@ -7890,13 +7954,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/ </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">彩 </t>
@@ -7906,6 +7971,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(cǎi)</t>
     </r>
@@ -7941,7 +8007,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">天文</t>
@@ -7951,13 +8017,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">金</t>
@@ -8023,13 +8090,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">mound, dam (</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">阝 </t>
@@ -8039,13 +8107,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">left) / city (</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">阝 </t>
@@ -8055,6 +8124,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">right)</t>
     </r>
@@ -8074,13 +8144,14 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dam (</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Noto Sans SC"/>
+        <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">阝 </t>
@@ -8090,6 +8161,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">left) / mound</t>
     </r>
@@ -8684,6 +8756,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -8705,10 +8778,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Noto Sans SC"/>
+      <name val="Noto Sans CJK SC"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -8850,50 +8924,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF5EB91E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBF819E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB3CAC7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFDE59"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -8958,40 +8988,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:U461"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G263" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A27" activeCellId="0" sqref="A1:F27"/>
+      <selection pane="bottomLeft" activeCell="A263" activeCellId="0" sqref="A263"/>
+      <selection pane="bottomRight" activeCell="H289" activeCellId="0" sqref="H289"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="4.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="4.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.36"/>
   </cols>

</xml_diff>